<commit_message>
modified concatenate code to write csv file
</commit_message>
<xml_diff>
--- a/data/raw/DOD_County_Shares_R.xlsx
+++ b/data/raw/DOD_County_Shares_R.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b19c66fe1ac65ec7/Documents/R/MEIS_Methodology/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{CCF9BE11-E262-455A-806C-E29CC29357F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EEDA30B-8566-4987-B9BD-2109C0C3A845}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{CCF9BE11-E262-455A-806C-E29CC29357F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8804C72B-4F41-4408-921C-36AC68FF37EF}"/>
   <bookViews>
     <workbookView xWindow="-18000" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1464,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2872,15 +2872,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="5aff56ac-f36b-49b3-8eea-e42fc37821cb">
@@ -2892,6 +2883,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3092,19 +3092,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61689470-BBC9-4AE0-9815-28B25381F91E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCD5482D-E383-4EEB-BB4E-A991C54640D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5aff56ac-f36b-49b3-8eea-e42fc37821cb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCD5482D-E383-4EEB-BB4E-A991C54640D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61689470-BBC9-4AE0-9815-28B25381F91E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5aff56ac-f36b-49b3-8eea-e42fc37821cb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>